<commit_message>
🚀 INITIAL COMMIT: AI Email Campaign Manager - The Most INSANE AI-Powered Email Marketing System Ever Built!
🔥 Features Added:
- 🤖 AI-Powered Email Responses with 4 Personality Types
- 📊 INSANE Analytics Dashboard with Real-time KPIs
- 🔄 Automated Follow-up Sequences with Sentiment Analysis
- 🧠 Smart Context Memory and Learning System
- ⚡ Real-time Email Monitoring and Auto-Reply
- 📈 Conversion Tracking and ROI Analytics
- 🎯 Sentiment Analysis and Intent Recognition
- 🔥 Production-Ready with Professional UI

This is not just a tool - it's a COMPLETE AI MARKETING MACHINE that works 24/7!

Built with ❤️ by HASHTECHVENTURES
The future of email marketing is here - and it's powered by AI! 🤖✨
</commit_message>
<xml_diff>
--- a/email_sender_datasource.xlsx
+++ b/email_sender_datasource.xlsx
@@ -1,104 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Customer Data" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sent Emails Data" sheetId="2" r:id="rId5"/>
+    <sheet name="Customer Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sent Emails Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>yourtestemail@gmail.com</t>
-  </si>
-  <si>
-    <t>TestA</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>TestB</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>zerobughero@gmail.com</t>
-  </si>
-  <si>
-    <t>TestC</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Sent Email</t>
-  </si>
-  <si>
-    <t>Sent Date</t>
-  </si>
-  <si>
-    <t>Sent Time</t>
-  </si>
-  <si>
-    <t>Sent Message</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <color theme="1"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <name val="Calibri"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="8"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
@@ -308,66 +244,67 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
       <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill/>
       </fill>
       <border/>
     </dxf>
@@ -402,51 +339,111 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="2">
-    <tableStyle count="3" pivot="0" name="Customer Data-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Customer Data-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="1"/>
+      <tableStyleElement type="firstRowStripe" dxfId="2"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="Sent Emails Data-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Sent Emails Data-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="1"/>
+      <tableStyleElement type="firstRowStripe" dxfId="2"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E9" displayName="Table1" name="Table1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E9" headerRowCount="1">
   <tableColumns count="5">
-    <tableColumn name="Email" id="1"/>
-    <tableColumn name="Last Name" id="2"/>
-    <tableColumn name="First Name" id="3"/>
-    <tableColumn name="Gender" id="4"/>
-    <tableColumn name="Status" id="5"/>
+    <tableColumn id="1" name="Email"/>
+    <tableColumn id="2" name="Last Name"/>
+    <tableColumn id="3" name="First Name"/>
+    <tableColumn id="4" name="Gender"/>
+    <tableColumn id="5" name="Status"/>
   </tableColumns>
-  <tableStyleInfo name="Customer Data-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Customer Data-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D10" displayName="Sent_Emails_Data" name="Sent_Emails_Data" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Sent_Emails_Data" displayName="Sent_Emails_Data" ref="A1:D10" headerRowCount="1">
   <tableColumns count="4">
-    <tableColumn name="Sent Email" id="1"/>
-    <tableColumn name="Sent Date" id="2"/>
-    <tableColumn name="Sent Time" id="3"/>
-    <tableColumn name="Sent Message" id="4"/>
+    <tableColumn id="1" name="Sent Email"/>
+    <tableColumn id="2" name="Sent Date"/>
+    <tableColumn id="3" name="Sent Time"/>
+    <tableColumn id="4" name="Sent Message"/>
   </tableColumns>
-  <tableStyleInfo name="Sent Emails Data-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Sent Emails Data-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -645,208 +642,335 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="FFEFEFEF"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="22.63"/>
+    <col width="22.63" customWidth="1" style="16" min="1" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5"/>
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>yourtestemail@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>TestA</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5"/>
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>test1@example.com</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>TestB</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="5"/>
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>test2@example.com</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>TestC</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="6" t="n"/>
+      <c r="B5" s="6" t="n"/>
+      <c r="C5" s="6" t="n"/>
+      <c r="D5" s="6" t="n"/>
+      <c r="E5" s="5" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="6" t="n"/>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="6" t="n"/>
+      <c r="D6" s="6" t="n"/>
+      <c r="E6" s="5" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="6" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="6" t="n"/>
+      <c r="D7" s="6" t="n"/>
+      <c r="E7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="6" t="n"/>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="6" t="n"/>
+      <c r="D8" s="6" t="n"/>
+      <c r="E8" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="6" t="n"/>
+      <c r="B9" s="6" t="n"/>
+      <c r="C9" s="6" t="n"/>
+      <c r="D9" s="6" t="n"/>
+      <c r="E9" s="7" t="n"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="FFD9EAD3"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.63"/>
-    <col customWidth="1" min="4" max="4" width="139.0"/>
+    <col width="22.63" customWidth="1" style="16" min="1" max="1"/>
+    <col width="139" customWidth="1" style="16" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sent Email</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Sent Date</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>Sent Time</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Sent Message</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>yourtestemail@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="C2" s="11" t="inlineStr">
+        <is>
+          <t>13:35:12</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sehr geehrte Frau TestA,
+Wir möchten Sie herzlich einladen, an unserer Umfrage teilzunehmen. 
+Ihre Meinung ist uns sehr wichtig!
+Hier finden Sie den Link zu der Umfrage: [Link to Survey]
+Mit freundlichen Grüßen,  
+Team Zerobughero
+</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t>yourtestemail@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="C3" s="11" t="inlineStr">
+        <is>
+          <t>13:35:17</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sehr geehrter Herr TestB,
+Wir möchten Sie herzlich einladen, an unserer Umfrage teilzunehmen. 
+Ihre Meinung ist uns sehr wichtig!
+Hier finden Sie den Link zu der Umfrage: [Link to Survey]
+Mit freundlichen Grüßen,  
+Team Zerobughero
+</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>zerobughero@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="C4" s="11" t="inlineStr">
+        <is>
+          <t>13:35:21</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guten Tag C TestC,
+Wir möchten Sie herzlich einladen, an unserer Umfrage teilzunehmen. 
+Ihre Meinung ist uns sehr wichtig!
+Hier finden Sie den Link zu der Umfrage: [Link to Survey]
+Mit freundlichen Grüßen,  
+Team Zerobughero
+</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="12"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
+      <c r="A5" s="12" t="n"/>
+      <c r="B5" s="10" t="n"/>
+      <c r="C5" s="11" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
+      <c r="A6" s="9" t="n"/>
+      <c r="B6" s="10" t="n"/>
+      <c r="C6" s="11" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="12"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
+      <c r="A7" s="12" t="n"/>
+      <c r="B7" s="10" t="n"/>
+      <c r="C7" s="11" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
+      <c r="A8" s="9" t="n"/>
+      <c r="B8" s="10" t="n"/>
+      <c r="C8" s="11" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="12"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
+      <c r="A9" s="12" t="n"/>
+      <c r="B9" s="10" t="n"/>
+      <c r="C9" s="11" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
+      <c r="A10" s="13" t="n"/>
+      <c r="B10" s="14" t="n"/>
+      <c r="C10" s="15" t="n"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>